<commit_message>
Cleaning file names, fixing df comparisons
</commit_message>
<xml_diff>
--- a/eligibility_model/code/offense_classification/county/los_angeles/selection_criteria.xlsx
+++ b/eligibility_model/code/offense_classification/county/los_angeles/selection_criteria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\3xProject\resentencing_data_initiative\eligibility_model\code\offense_classification\county\los_angeles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5347E512-0261-408E-BA8E-467F025C5DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE9B35B-524A-4F5D-9E54-0081748460C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -963,7 +963,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -974,12 +974,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor rgb="FFF4CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -995,7 +989,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1013,13 +1007,6 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1030,6 +1017,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1251,8 +1246,8 @@
   </sheetPr>
   <dimension ref="A1:C991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="E114" sqref="E114"/>
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
+      <selection activeCell="C306" sqref="C306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4584,102 +4579,102 @@
         <v>272</v>
       </c>
     </row>
-    <row r="303" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A303" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B303" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C303" s="10" t="s">
+    <row r="303" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A303" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B303" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C303" s="15" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="304" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A304" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B304" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C304" s="11" t="s">
+    <row r="304" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A304" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B304" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C304" s="17" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="305" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A305" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B305" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C305" s="11" t="s">
+    <row r="305" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A305" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B305" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C305" s="17" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="306" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A306" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B306" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C306" s="11" t="s">
+    <row r="306" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A306" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B306" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C306" s="17" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="307" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A307" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B307" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C307" s="11" t="s">
+    <row r="307" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A307" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B307" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C307" s="17" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="308" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A308" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B308" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C308" s="11" t="s">
+    <row r="308" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A308" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B308" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C308" s="17" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="309" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A309" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B309" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C309" s="11" t="s">
+    <row r="309" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A309" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B309" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C309" s="17" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="310" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A310" s="3" t="s">
+    <row r="310" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A310" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="B310" s="3" t="s">
+      <c r="B310" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="C310" s="4" t="s">
+      <c r="C310" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="311" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A311" s="3" t="s">
+    <row r="311" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A311" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="B311" s="3" t="s">
+      <c r="B311" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="C311" s="4" t="s">
+      <c r="C311" s="15" t="s">
         <v>282</v>
       </c>
     </row>
@@ -4728,68 +4723,68 @@
       </c>
     </row>
     <row r="316" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A316" s="12" t="s">
+      <c r="A316" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="B316" s="12" t="s">
+      <c r="B316" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C316" s="13" t="s">
+      <c r="C316" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A317" s="12" t="s">
+      <c r="A317" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="B317" s="12" t="s">
+      <c r="B317" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C317" s="14" t="s">
+      <c r="C317" s="11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A318" s="12" t="s">
+      <c r="A318" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="B318" s="12" t="s">
+      <c r="B318" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C318" s="14" t="s">
+      <c r="C318" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A319" s="12" t="s">
+      <c r="A319" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="B319" s="12" t="s">
+      <c r="B319" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C319" s="14" t="s">
+      <c r="C319" s="11" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="320" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A320" s="12" t="s">
+      <c r="A320" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="B320" s="12" t="s">
+      <c r="B320" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C320" s="14" t="s">
+      <c r="C320" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="321" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A321" s="12" t="s">
+      <c r="A321" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="B321" s="12" t="s">
+      <c r="B321" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C321" s="14" t="s">
+      <c r="C321" s="11" t="s">
         <v>286</v>
       </c>
     </row>
@@ -4797,22 +4792,22 @@
       <c r="C322" s="6"/>
     </row>
     <row r="323" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C323" s="14"/>
+      <c r="C323" s="11"/>
     </row>
     <row r="324" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C324" s="14"/>
+      <c r="C324" s="11"/>
     </row>
     <row r="325" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C325" s="14"/>
+      <c r="C325" s="11"/>
     </row>
     <row r="326" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C326" s="14"/>
+      <c r="C326" s="11"/>
     </row>
     <row r="327" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C327" s="14"/>
+      <c r="C327" s="11"/>
     </row>
     <row r="328" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C328" s="14"/>
+      <c r="C328" s="11"/>
     </row>
     <row r="329" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C329" s="4"/>
@@ -6824,20 +6819,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>287</v>
       </c>
     </row>
@@ -6865,12 +6860,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>289</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating selection criteria, remove PC190 offenses
</commit_message>
<xml_diff>
--- a/eligibility_model/code/offense_classification/county/los_angeles/selection_criteria.xlsx
+++ b/eligibility_model/code/offense_classification/county/los_angeles/selection_criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\3xProject\resentencing_data_initiative\eligibility_model\code\offense_classification\county\los_angeles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE9B35B-524A-4F5D-9E54-0081748460C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18D02A1-1A89-4047-AC7F-DB5AD26807AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="296">
   <si>
     <t>Table</t>
   </si>
@@ -910,6 +910,12 @@
   </si>
   <si>
     <t>273ab(b)</t>
+  </si>
+  <si>
+    <t>190(d)</t>
+  </si>
+  <si>
+    <t>190(c)</t>
   </si>
 </sst>
 </file>
@@ -989,7 +995,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1018,12 +1024,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1244,10 +1245,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C991"/>
+  <dimension ref="A1:C993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="C306" sqref="C306"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1881,7 +1882,7 @@
         <v>58</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>62</v>
+        <v>294</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1892,7 +1893,7 @@
         <v>58</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>63</v>
+        <v>295</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1903,7 +1904,7 @@
         <v>58</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1914,7 +1915,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1925,7 +1926,7 @@
         <v>58</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1936,7 +1937,7 @@
         <v>58</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1947,7 +1948,7 @@
         <v>58</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1958,7 +1959,7 @@
         <v>58</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1969,7 +1970,7 @@
         <v>58</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1980,7 +1981,7 @@
         <v>58</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1991,7 +1992,7 @@
         <v>58</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2001,8 +2002,8 @@
       <c r="B68" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>73</v>
+      <c r="C68" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2013,7 +2014,7 @@
         <v>58</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2024,7 +2025,7 @@
         <v>58</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2035,7 +2036,7 @@
         <v>58</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2045,8 +2046,8 @@
       <c r="B72" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C72" s="4" t="s">
-        <v>77</v>
+      <c r="C72" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2057,7 +2058,7 @@
         <v>58</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2068,7 +2069,7 @@
         <v>58</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2079,7 +2080,7 @@
         <v>58</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2090,7 +2091,7 @@
         <v>58</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2101,7 +2102,7 @@
         <v>58</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2112,7 +2113,7 @@
         <v>58</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2123,7 +2124,7 @@
         <v>58</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2134,7 +2135,7 @@
         <v>58</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2145,7 +2146,7 @@
         <v>58</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2156,7 +2157,7 @@
         <v>58</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2167,7 +2168,7 @@
         <v>58</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2178,7 +2179,7 @@
         <v>58</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2189,7 +2190,7 @@
         <v>58</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2200,7 +2201,7 @@
         <v>58</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2211,7 +2212,7 @@
         <v>58</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2222,7 +2223,7 @@
         <v>58</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2233,7 +2234,7 @@
         <v>58</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2244,7 +2245,7 @@
         <v>58</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2254,8 +2255,8 @@
       <c r="B91" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C91" s="5" t="s">
-        <v>95</v>
+      <c r="C91" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2266,7 +2267,7 @@
         <v>58</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2277,7 +2278,7 @@
         <v>58</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2287,8 +2288,8 @@
       <c r="B94" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C94" s="5" t="s">
-        <v>98</v>
+      <c r="C94" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2299,7 +2300,7 @@
         <v>58</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2310,7 +2311,7 @@
         <v>58</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2321,7 +2322,7 @@
         <v>58</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2332,7 +2333,7 @@
         <v>58</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2343,7 +2344,7 @@
         <v>58</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2354,7 +2355,7 @@
         <v>58</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2365,7 +2366,7 @@
         <v>58</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2376,7 +2377,7 @@
         <v>58</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2387,7 +2388,7 @@
         <v>58</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2398,7 +2399,7 @@
         <v>58</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2409,7 +2410,7 @@
         <v>58</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2420,7 +2421,7 @@
         <v>58</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2430,8 +2431,8 @@
       <c r="B107" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C107" s="4" t="s">
-        <v>111</v>
+      <c r="C107" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2441,8 +2442,8 @@
       <c r="B108" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C108" s="4" t="s">
-        <v>112</v>
+      <c r="C108" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2453,7 +2454,7 @@
         <v>58</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2464,7 +2465,7 @@
         <v>58</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2475,7 +2476,7 @@
         <v>58</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2486,7 +2487,7 @@
         <v>58</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>293</v>
+        <v>114</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2497,7 +2498,7 @@
         <v>58</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>290</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2508,7 +2509,7 @@
         <v>58</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>116</v>
+        <v>293</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2519,7 +2520,7 @@
         <v>58</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>117</v>
+        <v>290</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2530,7 +2531,7 @@
         <v>58</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2541,7 +2542,7 @@
         <v>58</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2552,7 +2553,7 @@
         <v>58</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2563,7 +2564,7 @@
         <v>58</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2574,7 +2575,7 @@
         <v>58</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2585,7 +2586,7 @@
         <v>58</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2596,7 +2597,7 @@
         <v>58</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2607,7 +2608,7 @@
         <v>58</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2618,7 +2619,7 @@
         <v>58</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2629,7 +2630,7 @@
         <v>58</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2640,7 +2641,7 @@
         <v>58</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2651,7 +2652,7 @@
         <v>58</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2662,7 +2663,7 @@
         <v>58</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2673,7 +2674,7 @@
         <v>58</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2684,7 +2685,7 @@
         <v>58</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2695,7 +2696,7 @@
         <v>58</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2706,7 +2707,7 @@
         <v>58</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>291</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2717,7 +2718,7 @@
         <v>58</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>292</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2728,29 +2729,29 @@
         <v>58</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>134</v>
+        <v>291</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>136</v>
+        <v>58</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>59</v>
+        <v>292</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>136</v>
+        <v>58</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2761,7 +2762,7 @@
         <v>136</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2772,7 +2773,7 @@
         <v>136</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2783,7 +2784,7 @@
         <v>136</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>138</v>
+        <v>76</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2794,7 +2795,7 @@
         <v>136</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>139</v>
+        <v>77</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2805,7 +2806,7 @@
         <v>136</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2816,7 +2817,7 @@
         <v>136</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2827,7 +2828,7 @@
         <v>136</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2838,7 +2839,7 @@
         <v>136</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2849,7 +2850,7 @@
         <v>136</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2860,7 +2861,7 @@
         <v>136</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2871,7 +2872,7 @@
         <v>136</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2882,7 +2883,7 @@
         <v>136</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2893,7 +2894,7 @@
         <v>136</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2904,7 +2905,7 @@
         <v>136</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2915,7 +2916,7 @@
         <v>136</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2926,7 +2927,7 @@
         <v>136</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2937,7 +2938,7 @@
         <v>136</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2948,7 +2949,7 @@
         <v>136</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2959,7 +2960,7 @@
         <v>136</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2970,7 +2971,7 @@
         <v>136</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2981,7 +2982,7 @@
         <v>136</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2992,7 +2993,7 @@
         <v>136</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3003,7 +3004,7 @@
         <v>136</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3014,7 +3015,7 @@
         <v>136</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3025,7 +3026,7 @@
         <v>136</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3036,7 +3037,7 @@
         <v>136</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3047,7 +3048,7 @@
         <v>136</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3058,7 +3059,7 @@
         <v>136</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3069,7 +3070,7 @@
         <v>136</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3080,7 +3081,7 @@
         <v>136</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3091,29 +3092,29 @@
         <v>136</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3124,7 +3125,7 @@
         <v>157</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3135,7 +3136,7 @@
         <v>157</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3146,7 +3147,7 @@
         <v>157</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>76</v>
+        <v>160</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3157,7 +3158,7 @@
         <v>157</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3168,7 +3169,7 @@
         <v>157</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>163</v>
+        <v>76</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3179,7 +3180,7 @@
         <v>157</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3190,7 +3191,7 @@
         <v>157</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3201,7 +3202,7 @@
         <v>157</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3212,7 +3213,7 @@
         <v>157</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3223,7 +3224,7 @@
         <v>157</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3234,7 +3235,7 @@
         <v>157</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3245,7 +3246,7 @@
         <v>157</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>78</v>
+        <v>167</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3256,7 +3257,7 @@
         <v>157</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3267,7 +3268,7 @@
         <v>157</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>170</v>
+        <v>78</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3278,7 +3279,7 @@
         <v>157</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3289,7 +3290,7 @@
         <v>157</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3300,7 +3301,7 @@
         <v>157</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3311,7 +3312,7 @@
         <v>157</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3322,7 +3323,7 @@
         <v>157</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3333,7 +3334,7 @@
         <v>157</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3344,7 +3345,7 @@
         <v>157</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3355,7 +3356,7 @@
         <v>157</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3366,7 +3367,7 @@
         <v>157</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3377,7 +3378,7 @@
         <v>157</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3388,7 +3389,7 @@
         <v>157</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3399,7 +3400,7 @@
         <v>157</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3410,7 +3411,7 @@
         <v>157</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3421,7 +3422,7 @@
         <v>157</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3432,7 +3433,7 @@
         <v>157</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3443,7 +3444,7 @@
         <v>157</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3454,7 +3455,7 @@
         <v>157</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3465,7 +3466,7 @@
         <v>157</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3476,7 +3477,7 @@
         <v>157</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3487,7 +3488,7 @@
         <v>157</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3498,7 +3499,7 @@
         <v>157</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>112</v>
+        <v>189</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3509,7 +3510,7 @@
         <v>157</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3520,7 +3521,7 @@
         <v>157</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>192</v>
+        <v>112</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3531,7 +3532,7 @@
         <v>157</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>113</v>
+        <v>191</v>
       </c>
     </row>
     <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3542,7 +3543,7 @@
         <v>157</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>114</v>
+        <v>192</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3553,7 +3554,7 @@
         <v>157</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>193</v>
+        <v>113</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3564,7 +3565,7 @@
         <v>157</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>194</v>
+        <v>114</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3575,7 +3576,7 @@
         <v>157</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3586,7 +3587,7 @@
         <v>157</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3597,7 +3598,7 @@
         <v>157</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3608,7 +3609,7 @@
         <v>157</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3619,7 +3620,7 @@
         <v>157</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3630,7 +3631,7 @@
         <v>157</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3641,7 +3642,7 @@
         <v>157</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3652,7 +3653,7 @@
         <v>157</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3663,7 +3664,7 @@
         <v>157</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3674,7 +3675,7 @@
         <v>157</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3685,7 +3686,7 @@
         <v>157</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3696,7 +3697,7 @@
         <v>157</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3707,7 +3708,7 @@
         <v>157</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3718,7 +3719,7 @@
         <v>157</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3729,7 +3730,7 @@
         <v>157</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3740,7 +3741,7 @@
         <v>157</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3751,7 +3752,7 @@
         <v>157</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>123</v>
+        <v>208</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3762,7 +3763,7 @@
         <v>157</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>209</v>
+        <v>122</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3773,7 +3774,7 @@
         <v>157</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>210</v>
+        <v>123</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3784,7 +3785,7 @@
         <v>157</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3795,7 +3796,7 @@
         <v>157</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3806,7 +3807,7 @@
         <v>157</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3817,7 +3818,7 @@
         <v>157</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3828,7 +3829,7 @@
         <v>157</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3839,7 +3840,7 @@
         <v>157</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3850,7 +3851,7 @@
         <v>157</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3861,7 +3862,7 @@
         <v>157</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>144</v>
+        <v>216</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3872,7 +3873,7 @@
         <v>157</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>124</v>
+        <v>217</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3883,7 +3884,7 @@
         <v>157</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3894,7 +3895,7 @@
         <v>157</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
     </row>
     <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3905,7 +3906,7 @@
         <v>157</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>218</v>
+        <v>145</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3916,7 +3917,7 @@
         <v>157</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>219</v>
+        <v>146</v>
       </c>
     </row>
     <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3927,7 +3928,7 @@
         <v>157</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3938,7 +3939,7 @@
         <v>157</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3949,7 +3950,7 @@
         <v>157</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3960,7 +3961,7 @@
         <v>157</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3971,7 +3972,7 @@
         <v>157</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>126</v>
+        <v>222</v>
       </c>
     </row>
     <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3982,7 +3983,7 @@
         <v>157</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>147</v>
+        <v>223</v>
       </c>
     </row>
     <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3993,7 +3994,7 @@
         <v>157</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>224</v>
+        <v>126</v>
       </c>
     </row>
     <row r="250" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4004,7 +4005,7 @@
         <v>157</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>225</v>
+        <v>147</v>
       </c>
     </row>
     <row r="251" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4015,7 +4016,7 @@
         <v>157</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>127</v>
+        <v>224</v>
       </c>
     </row>
     <row r="252" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4026,7 +4027,7 @@
         <v>157</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4037,7 +4038,7 @@
         <v>157</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>227</v>
+        <v>127</v>
       </c>
     </row>
     <row r="254" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4048,7 +4049,7 @@
         <v>157</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="255" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4059,7 +4060,7 @@
         <v>157</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="256" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4070,7 +4071,7 @@
         <v>157</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="257" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4081,7 +4082,7 @@
         <v>157</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="258" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4092,7 +4093,7 @@
         <v>157</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="259" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4103,7 +4104,7 @@
         <v>157</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="260" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4114,7 +4115,7 @@
         <v>157</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="261" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4125,7 +4126,7 @@
         <v>157</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4136,7 +4137,7 @@
         <v>157</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="263" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4147,7 +4148,7 @@
         <v>157</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="264" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4158,7 +4159,7 @@
         <v>157</v>
       </c>
       <c r="C264" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="265" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4169,7 +4170,7 @@
         <v>157</v>
       </c>
       <c r="C265" s="4" t="s">
-        <v>128</v>
+        <v>237</v>
       </c>
     </row>
     <row r="266" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4180,7 +4181,7 @@
         <v>157</v>
       </c>
       <c r="C266" s="4" t="s">
-        <v>129</v>
+        <v>238</v>
       </c>
     </row>
     <row r="267" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4191,7 +4192,7 @@
         <v>157</v>
       </c>
       <c r="C267" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="268" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4202,7 +4203,7 @@
         <v>157</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>239</v>
+        <v>129</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4213,7 +4214,7 @@
         <v>157</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>240</v>
+        <v>130</v>
       </c>
     </row>
     <row r="270" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4224,7 +4225,7 @@
         <v>157</v>
       </c>
       <c r="C270" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="271" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4235,7 +4236,7 @@
         <v>157</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4246,7 +4247,7 @@
         <v>157</v>
       </c>
       <c r="C272" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="273" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4257,7 +4258,7 @@
         <v>157</v>
       </c>
       <c r="C273" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="274" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4268,7 +4269,7 @@
         <v>157</v>
       </c>
       <c r="C274" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="275" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4279,7 +4280,7 @@
         <v>157</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4290,7 +4291,7 @@
         <v>157</v>
       </c>
       <c r="C276" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="277" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4301,7 +4302,7 @@
         <v>157</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4312,7 +4313,7 @@
         <v>157</v>
       </c>
       <c r="C278" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="279" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4323,7 +4324,7 @@
         <v>157</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>131</v>
+        <v>248</v>
       </c>
     </row>
     <row r="280" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4334,7 +4335,7 @@
         <v>157</v>
       </c>
       <c r="C280" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="281" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4345,7 +4346,7 @@
         <v>157</v>
       </c>
       <c r="C281" s="4" t="s">
-        <v>251</v>
+        <v>131</v>
       </c>
     </row>
     <row r="282" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4356,7 +4357,7 @@
         <v>157</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4367,7 +4368,7 @@
         <v>157</v>
       </c>
       <c r="C283" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="284" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4378,7 +4379,7 @@
         <v>157</v>
       </c>
       <c r="C284" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="285" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4389,7 +4390,7 @@
         <v>157</v>
       </c>
       <c r="C285" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="286" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4400,7 +4401,7 @@
         <v>157</v>
       </c>
       <c r="C286" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="287" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4411,7 +4412,7 @@
         <v>157</v>
       </c>
       <c r="C287" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="288" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4422,7 +4423,7 @@
         <v>157</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="289" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4433,7 +4434,7 @@
         <v>157</v>
       </c>
       <c r="C289" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="290" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4444,7 +4445,7 @@
         <v>157</v>
       </c>
       <c r="C290" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4455,7 +4456,7 @@
         <v>157</v>
       </c>
       <c r="C291" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4466,7 +4467,7 @@
         <v>157</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="293" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4477,7 +4478,7 @@
         <v>157</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="294" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4488,7 +4489,7 @@
         <v>157</v>
       </c>
       <c r="C294" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="295" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4499,7 +4500,7 @@
         <v>157</v>
       </c>
       <c r="C295" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="296" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4510,7 +4511,7 @@
         <v>157</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4521,7 +4522,7 @@
         <v>157</v>
       </c>
       <c r="C297" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4532,7 +4533,7 @@
         <v>157</v>
       </c>
       <c r="C298" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4543,7 +4544,7 @@
         <v>157</v>
       </c>
       <c r="C299" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4553,8 +4554,8 @@
       <c r="B300" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C300" s="6" t="s">
-        <v>270</v>
+      <c r="C300" s="4" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4564,8 +4565,8 @@
       <c r="B301" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C301" s="7" t="s">
-        <v>271</v>
+      <c r="C301" s="4" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="302" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4575,107 +4576,107 @@
       <c r="B302" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C302" s="8" t="s">
+      <c r="C302" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A303" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B303" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C303" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A304" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B304" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C304" s="8" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="303" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A303" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B303" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C303" s="15" t="s">
+    <row r="305" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A305" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B305" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C305" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="304" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A304" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B304" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C304" s="17" t="s">
+    <row r="306" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A306" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B306" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C306" s="14" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="305" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A305" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B305" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C305" s="17" t="s">
+    <row r="307" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A307" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B307" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C307" s="14" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="306" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A306" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B306" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C306" s="17" t="s">
+    <row r="308" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A308" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B308" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C308" s="14" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="307" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A307" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B307" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C307" s="17" t="s">
+    <row r="309" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A309" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B309" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C309" s="14" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="308" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A308" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B308" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C308" s="17" t="s">
+    <row r="310" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A310" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B310" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C310" s="14" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="309" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A309" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B309" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C309" s="17" t="s">
+    <row r="311" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A311" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B311" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C311" s="14" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A310" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="B310" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="C310" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A311" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="B311" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="C311" s="15" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="312" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4686,7 +4687,7 @@
         <v>281</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4697,7 +4698,7 @@
         <v>281</v>
       </c>
       <c r="C313" s="4" t="s">
-        <v>61</v>
+        <v>282</v>
       </c>
     </row>
     <row r="314" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4708,7 +4709,7 @@
         <v>281</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="315" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4719,29 +4720,29 @@
         <v>281</v>
       </c>
       <c r="C315" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A316" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B316" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C316" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A317" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B317" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C317" s="4" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="316" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A316" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="B316" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="C316" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="317" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A317" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="B317" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="C317" s="11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4751,8 +4752,8 @@
       <c r="B318" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C318" s="11" t="s">
-        <v>72</v>
+      <c r="C318" s="10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4763,7 +4764,7 @@
         <v>284</v>
       </c>
       <c r="C319" s="11" t="s">
-        <v>285</v>
+        <v>71</v>
       </c>
     </row>
     <row r="320" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4774,7 +4775,7 @@
         <v>284</v>
       </c>
       <c r="C320" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="321" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4785,17 +4786,33 @@
         <v>284</v>
       </c>
       <c r="C321" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A322" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="B322" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="C322" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A323" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="B323" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="C323" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="322" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C322" s="6"/>
-    </row>
-    <row r="323" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C323" s="11"/>
-    </row>
     <row r="324" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C324" s="11"/>
+      <c r="C324" s="6"/>
     </row>
     <row r="325" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C325" s="11"/>
@@ -4810,10 +4827,10 @@
       <c r="C328" s="11"/>
     </row>
     <row r="329" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C329" s="4"/>
+      <c r="C329" s="11"/>
     </row>
     <row r="330" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C330" s="4"/>
+      <c r="C330" s="11"/>
     </row>
     <row r="331" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C331" s="4"/>
@@ -5233,10 +5250,10 @@
       <c r="C469" s="4"/>
     </row>
     <row r="470" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C470" s="5"/>
+      <c r="C470" s="4"/>
     </row>
     <row r="471" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C471" s="5"/>
+      <c r="C471" s="4"/>
     </row>
     <row r="472" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C472" s="5"/>
@@ -6797,6 +6814,12 @@
     </row>
     <row r="991" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C991" s="5"/>
+    </row>
+    <row r="992" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C992" s="5"/>
+    </row>
+    <row r="993" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C993" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update selection criteria with subsection penal codes for robberies
</commit_message>
<xml_diff>
--- a/eligibility_model/code/offense_classification/county/los_angeles/selection_criteria.xlsx
+++ b/eligibility_model/code/offense_classification/county/los_angeles/selection_criteria.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="300">
   <si>
     <t>Table</t>
   </si>
@@ -897,6 +897,18 @@
   </si>
   <si>
     <t>211A</t>
+  </si>
+  <si>
+    <t>666</t>
+  </si>
+  <si>
+    <t>666.5</t>
+  </si>
+  <si>
+    <t>666.5(a)</t>
+  </si>
+  <si>
+    <t>666(a)</t>
   </si>
   <si>
     <t>None pending as of 10/2/2023</t>
@@ -963,7 +975,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -985,6 +997,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -4771,33 +4789,107 @@
       </c>
     </row>
     <row r="324" ht="15.75" customHeight="1">
-      <c r="C324" s="6"/>
+      <c r="A324" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B324" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C324" s="10" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="325" ht="15.75" customHeight="1">
-      <c r="C325" s="4"/>
+      <c r="A325" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B325" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C325" s="11" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="326" ht="15.75" customHeight="1">
-      <c r="C326" s="4"/>
+      <c r="A326" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B326" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C326" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="327" ht="15.75" customHeight="1">
-      <c r="C327" s="4"/>
+      <c r="A327" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B327" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C327" s="11" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="328" ht="15.75" customHeight="1">
-      <c r="C328" s="4"/>
+      <c r="A328" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B328" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C328" s="11" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="329" ht="15.75" customHeight="1">
-      <c r="C329" s="4"/>
+      <c r="A329" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B329" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C329" s="11" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="330" ht="15.75" customHeight="1">
-      <c r="C330" s="4"/>
+      <c r="A330" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B330" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C330" s="11" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="331" ht="15.75" customHeight="1">
-      <c r="C331" s="4"/>
+      <c r="A331" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B331" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C331" s="11" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="332" ht="15.75" customHeight="1">
-      <c r="C332" s="4"/>
+      <c r="A332" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B332" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C332" s="11" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="333" ht="15.75" customHeight="1">
+      <c r="A333" s="3"/>
+      <c r="B333" s="3"/>
       <c r="C333" s="4"/>
     </row>
     <row r="334" ht="15.75" customHeight="1">
@@ -6818,7 +6910,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5">
@@ -6848,13 +6940,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="81.75" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>294</v>
+      <c r="A1" s="12" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="s">
-        <v>295</v>
+      <c r="A2" s="12" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>